<commit_message>
PDF extraction and DB population
</commit_message>
<xml_diff>
--- a/Datascraping/output_excel_files_new/Aligarh Muslim University_tables.xlsx
+++ b/Datascraping/output_excel_files_new/Aligarh Muslim University_tables.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,32 +520,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UG [4 Years Program(s)]</t>
+          <t>UG [5 Years Program(s)]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>240</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>240</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>240</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>240</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>220</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>325</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -710,68 +710,68 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UG [4 Years+          <t>UG [5 Years Program(s)]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1552</t>
+          <t>706</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>328</t>
+          <t>393</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1880</t>
+          <t>1099</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1482</t>
+          <t>487</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>607</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>568</t>
+          <t>35</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>363</t>
+          <t>192</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>207</t>
         </is>
       </c>
     </row>
@@ -784,47 +784,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>475</t>
+          <t>43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>33</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>552</t>
+          <t>76</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>442</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>195</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -916,24 +916,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2015-16</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>2016-17</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>385</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>424</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2017-18</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>0</t>
@@ -946,22 +946,23 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>220</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>169</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>500000(Five Lacs)</t>
+          <t>980000( Nine Lacs+Eighty Thousand Only)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>32</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -971,24 +972,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>2016-17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>2017-18</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>385</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>438</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2018-19</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>0</t>
@@ -1001,23 +1002,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>219</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>179</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>562000(Five Lacs-Sixty two thousand)</t>
+          <t>1020000(Ten Lacs+Twenty Thousand Only+)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>26</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1027,24 +1029,24 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>2017-18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>2018-19</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>365</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>424</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2019-20</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>0</t>
@@ -1057,23 +1059,23 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>385</t>
+          <t>219</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>181</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>550000(Five Lacs fifty-thousand)</t>
+          <t>1230000(Twelve Lacs+Thirty  Thousand Only)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>32</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1146,12 +1148,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>261</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1161,24 +1163,23 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>388000(Three Lacs-Eighty Eight-Thousand)</t>
+          <t>980000(Nine Lacs+Eighty Thousand Only)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -1195,12 +1196,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1210,23 +1211,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>475000(Four Lacs-seventy five thousand)</t>
+          <t>1020000(Ten Lacs+Twenty Thousand Only+)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1243,12 +1245,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1258,23 +1260,23 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>475000(Four Lacs-seventy five thousand)</t>
+          <t>1032000(Ten Lacs+Thirty Two thousand)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1329,7 +1331,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>242</t>
+          <t>77</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1352,7 +1354,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1421,17 +1423,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1462,7 +1464,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1555,25 +1557,24 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Library ( Books, Journals and e-Resources only)</t>
+          <t>Library</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4680936 (Forty six lacs  eighty thousand nine hundred thirty-six)</t>
+          <t>723189 (Seven Lacs Twenty Three Thousand One Hundred+Eighty Nine Only)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>9218238 (Ninty two lacs eighteen thousand two hundred thirty-eight)</t>
+          <t>1040996 (Ten Lacs Forty Thousand Nine Hundred Ninety Six)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6476881 (Sixty Four lacs Seventy six Thousand Eight hundred-Eighty one)</t>
+          <t>1294847 (Twelve Lacs Ninety Four Thousand Eight Hundred+Forty Seven )</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1589,24 +1590,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>New Equipment and software for Laboratories</t>
+          <t>New Equipment for Laboratories</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11085181 (One Crore Ten lacs Eighty five thousand one-hundred eighty one)</t>
+          <t>18900 (Eighteen Thousand Nine Hundred Only)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>8444022 (Eighty four lacs forty four thousand twenty two)</t>
+          <t>0 (Zero)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>16196188 (One crore Sixty one Lacs Ninty six thousand One-hundred Eighty eight)</t>
+          <t>0 (Zero)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1622,22 +1621,25 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Engineering Workshops</t>
+          <t>Other expenditure on creation of Capital Assets (excluding+expenditure on Land and Building)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1060846 (Ten lacs sixty thousand eight hundred forty six)</t>
+          <t>749190 (Seven Lacs Forty Nine Thousand one Hundred Ninty+Only)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1001829 (Ten lacs one thousand eight hundred twenty nine)</t>
+          <t>1067567 (Ten Lacs Sixty  Seven Thousand Five Hundred Sixty+Seven Only)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1150304 (Eleven lacs Fifty thousand three hundred four)</t>
+          <t>275500 (Two Lacs Seventy Five Thousand Five Hundred Only)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1653,27 +1655,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Other expenditure on creation of Capital Assets (For setting up-classrooms, seminar hall, conference hall , library, Lab, Engg-workshops excluding expenditure on Land and Building)</t>
+          <t>Financial Year</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5913672 (Fifty nine lacs thirteen thousand six hundred seventy-two)</t>
+          <t>2021-22</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>7259665 (Seventy two lacs fifty nine thousand six hundred-sixty five)</t>
+          <t>2020-21</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5693629 (Fifty six lacs Ninty three thousand Six hundred-twenty nine)</t>
+          <t>2019-20</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1687,24 +1684,20 @@
       <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Financial Year</t>
-        </is>
-      </c>
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2021-22</t>
+          <t>Utilised Amount</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2020-21</t>
+          <t>Utilised Amount</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2019-20</t>
+          <t>Utilised Amount</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1718,22 +1711,14 @@
       <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Utilised Amount</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Utilised Amount</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Utilised Amount</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Annual Operational Expenditure</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -1747,12 +1732,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Annual Operational Expenditure</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+          <t>Salaries (Teaching and Non Teaching staff)</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>94630208 (Nine Crores  Forty Six Lacs Thirty Thousand Two+Hundred Eight Only)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>81941486 (Eight Crores Nineteen Lacs Forty One Thousand+Four Hundred Eighty Six Only )</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>63611508 (Six Crores Thirty Six Lacs Eleven Thousand Five+Hundred Eight Only)</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1766,25 +1766,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Salaries (Teaching and Non Teaching staff)</t>
+          <t>Maintenance of Academic Infrastructure or consumables and+other running expenditures(excluding maintenance of hostels+and allied services,rent of the building, depreciation cost, etc)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1056068812 (One hundred five crores sixty lacs sixty eight-thousand eight hundred twelve)</t>
+          <t>971100 (Nine Lacs Seventy One Thousand One Hundred+Only)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>710373148 (Seventy one crores three lacs seventy three-thousand one hundred forty eight)</t>
+          <t>1213250 (Twelve Lacs Thirteen Thousand Two Hundred Fifty+Only)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>978459886 (Ninty seven crores Eighty four Lacs Fifty nine-thousand eight hundred Eighty six)</t>
+          <t>1029513 (Ten Lacs Twenty Nine Thousand Five Hundred+thirteen Only)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1800,26 +1802,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Maintenance of Academic Infrastructure or consumables and-other running expenditures(excluding maintenance of hostels-and allied services,rent of the building, depreciation cost, etc)</t>
+          <t>Seminars/Conferences/Workshops</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>26717370 (Two crores sixty seven lacs seventeen thousand-three hundred seventy)</t>
+          <t>250000 (Two Lacs Fifty Thousand )</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4690405 (Forty six lacs ninty thousand four hundred five)</t>
+          <t>425000 (Four Lacs Twenty Five  Thousand Only)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2029485 (Twenty lacs Twenty Nine Thousand Four hundred-Eighty five)</t>
+          <t>278000 (Two Lacs Seventy Eight Thousand Only)</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1835,25 +1833,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Seminars/Conferences/Workshops</t>
+          <t>Financial Year</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>393538 (Three lacs ninty three thousand five hundred thirty-eight)</t>
+          <t>2021-22</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>428898 (Four Lacs twenty eight thousand eight hundred ninty-eight)</t>
+          <t>2020-21</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1339194 (Thirteen Lacs Thirty nine thousand One hundred-Ninty four)</t>
+          <t>2019-20</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1869,22 +1864,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Financial Year</t>
+          <t>Total no. of Sponsored Projects</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2021-22</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2020-21</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2019-20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1900,22 +1895,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Total no. of Sponsored Projects</t>
+          <t>Total no. of Funding Agencies</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1931,22 +1926,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Total no. of Funding Agencies</t>
+          <t>Total Amount Received (Amount in Rupees)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>250000</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1962,22 +1957,22 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Total Amount Received (Amount in Rupees)</t>
+          <t>Amount Received in Words</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>107488000</t>
+          <t>Two Lacs Fifty Thousand Only</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>204973105</t>
+          <t>Zero</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>20802384</t>
+          <t>Zero</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1993,23 +1988,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Amount Received in Words</t>
+          <t>Financial Year</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ten crores seventy four lacs eighty eight thousand</t>
+          <t>2021-22</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Twenty crores forty nine lacs seventy three thousand one-hundred five</t>
+          <t>2020-21</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Two Crore Eight Lacs two thousand Three hundred Eighty four</t>
+          <t>2019-20</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -2025,22 +2019,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Financial Year</t>
+          <t>Total no. of Consultancy Projects</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2021-22</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2020-21</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2019-20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -2056,22 +2050,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Total no. of Consultancy Projects</t>
+          <t>Total no. of Client Organizations</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -2087,22 +2081,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Total no. of Client Organizations</t>
+          <t>Total Amount Received (Amount in Rupees)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -2118,22 +2112,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Total Amount Received (Amount in Rupees)</t>
+          <t>Amount Received in Words</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>20859628</t>
+          <t>Zero</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>34578039</t>
+          <t>Zero</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>20372779</t>
+          <t>Zero</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -2149,26 +2143,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Amount Received in Words</t>
+          <t>1. Do your institution buildings have Lifts/Ramps?</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Two crores eight lacs fifty nine thousand six hundred twenty-eight</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Three crores forty five lacs seventy eight thousand thirty nine</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Two crore Three Lacs Seventy two Thousand Seven hundred-Seventy Nine</t>
-        </is>
-      </c>
+          <t>Yes, more than 80% of the buildings</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -2182,12 +2166,13 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1. Do your institution buildings have Lifts/Ramps?</t>
+          <t>2. Do your institution have provision for walking aids, including wheelchairs and transportation from one building to another for+handicapped students?</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Yes, more than 80% of the buildings</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -2205,13 +2190,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2. Do your institution have provision for walking aids, including wheelchairs and transportation from one building to another for-handicapped students?</t>
+          <t>3. Do your institution buildings have specially designed toilets for handicapped students?</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Yes, more than 80% of the buildings</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -2229,12 +2213,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>3. Do your institution buildings have specially designed toilets for handicapped students?</t>
+          <t>Number of faculty members entered</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Yes, more than 80% of the buildings</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -2249,29 +2233,6 @@
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Number of faculty members entered</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>233</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>